<commit_message>
Ajuste na janela, pegar informações sobre vaga desejada
</commit_message>
<xml_diff>
--- a/vagas.xlsx
+++ b/vagas.xlsx
@@ -446,22 +446,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DESENVOLVEDOR DE HARDWARE AUTOMOMOTIVO PLENO | HÍBRIDO (Curitiba)</t>
+          <t>Analista de testes</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mobi7 Localiza</t>
+          <t>Formel D Group</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Curitiba, Paraná, Brasil (Híbrido)</t>
+          <t>Hortolândia, São Paulo, Brasil (Presencial)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4314908154/?eBP=CwEAAAGaAxqMylJH1eywLIcn-V_HvJZ6x_89_-Vrn4maqZKVkShkvWChQ7ejzc07Gc1xGTwhM1Oi00_C26KcCVfqvGv2Rojx2dUg5axLgCs1hLen5liodZn3vqY_FdWdlir3DSDgdwfeJcFUAFcv6cNfPCNMB6Ga9un5YyRVe29ejIeogSDAsJjJeLQ5uOkMQ8kvmg1CG72weDoyLWMYevfwBXwbmTH5gs5FqFCCT9PpQH43xIQ1qrgfOPgn3GSpBscXc8cs_9BNIAShTvwnKCHBLMbN9EjzXM4T2pzSfuX3OGvLQMa3GryoLX7jGgkvDxYT5_P4dPIFZWQWNR0UJ5ivyuoRApLwzB3zDSl9RKPUMUbgyBb6xT8g0m-2zhpcKi5aRFTOuzXh0kyf_fiekjet_JxpruXvwyi5rDVFUYT88i_gTzU6yIDXXG3ZVnsHheQCbi_6Xp1DE9MJE7NRmv08MUtLWur_40o-V8GO84kX73O8ZjVzY-t1wh1Yr7cujKvZ394v0dM&amp;refId=KljewT48X7gbgzXncwajHQ%3D%3D&amp;trackingId=PDYz4R9mIHjE7HMKhqXBeg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4316648699/?eBP=CwEAAAGaA23jKkNVExKLwjxHAGBjA50PWwQJm7Fx7DdiqH5mJxphN1TKt0y7jv0VYFvbyMBbvJqsZtfUeyvh8d0ph8RXLVSQcqdr3x999G6qgGUtH9LP2vJQlBTqN7g37g_MV0VhCppQCToYRu1kIgYZSE0XbdCJ3ldH8EpmdU4kym7dyEe21jvE325Fy2VCxL-3GJ2-DYEHjKAsrS09ONHDpNKIFZvrxsuwnaVv18dUzYgav22RAY6VjDDarDKxaNQ8BbIfXxjLE_wA1Yorw2cfeQtESNDhsAj89ux6_j1Mih0PXqEv-aQvHPqdPmtw0nXOaRtE2OsGKcDDnW7OMe1AFxjK_6HSGQmaO9_csyUDtW1cHk0BK-lTtQtIE6HdvXiAXSSJFSEZssFdxcd_fcjnQ03e1sSyp21WrCCf1-9jTc_yPkJw9jzfSaENFQkbVkt9EqfSqnUxNofSVp_4aTo8FMF18GV2E9JS3TiszLgwpo1hUpDlXB_zpLBo24fOd6EU6yjmZaiRjA&amp;refId=lbnt2cNJFf5kM%2FxHsC7d9A%3D%3D&amp;trackingId=mLqNvWqSBSK%2Bh32dgP%2B6Pg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>
@@ -483,29 +483,29 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4292388244/?eBP=CwEAAAGaAxqMy_lQSIoYpub6Nd32TueiY6Zcr2aHrRtGT3ZmzDF03nXt7IajOp-XCGVytfogrF8jUNF_AZgRg9EHgork2VasqWQPKTwxUAFS3DnrSN0ZNHjFZzNqdcZXmhodOAQ9dGp5VN_tkvBTXUPhBI9t5w8lIM2WYpVfgMYLDtP_cKM9tB1-CRl7zZ1VWK5DfIqX5nvUh_UUY5zC4Zz1PyBA03y5r9yE_Kpq1YU4iyNb2aQdBD-ajP-fMjs6LnZiUgXLBsahHJZCBqtI7kZI_3XE_w1yQSXCfYhM0m3IbyXAM48W3ZB5YoIwwxG5XDgjAI38YWAYCh7tD-wzkn0xgD42YzwVwQbG0RBGNjK0vV00SAm0OFDBRGsn3MHjLA_yoglLmM_mCdD7OGa5CYfIVvkAXsmIpPaU5Cy-U3KQce-5MqtYrQBbhAOflpPxwPleDX53TjaVekQAO6thw4Ij3DnAtyXFl6NNfYXpfKH1Qd9Zd95L-_BY8Npw-qz6zAiJOj0Q7tI&amp;refId=KljewT48X7gbgzXncwajHQ%3D%3D&amp;trackingId=3OXj86Ktyvs1I%2FWN14aEFw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4292388244/?eBP=CwEAAAGaA23jKorieug2KzePpeTJ7QXoTad1BS_QJ19ZUFkjZPY7OWIf9c4SPEYwowLkRc6jxa_qmbcCVLJBDtzEnt_vjTVHyYu_A8ycyYaUWmZb4rsPrOJxrtjE2M4MwlA7QyqtMhRK5dGPBTG9veazgdrGbzlFK0tO02wNFBLEH_43arEoyoHnfb2IVC7poVirYtU6MA3swkUc0w8ZJ5UtBGWCWCs5QP5VwU5dwN98_q9hD51txfyda4gBu1epLS937zaNjRmLJ87aaPYY_UEehAYVe5QAzP0QRnrvkglxwaH2McacNa20P_Ac7iCrO15kbq3qnZnsxo2-pisvPsVdo2JDsUG3FS1Y5e-IqkBwI_RA0Imd-rNbOPfPEiW05X6ZwT4_rZlqESj55MamLAJe64TkV6-6l9T3q4fjc4xfUrjcFzGodM0qU-UZ9jPghVpSvx06yfbZyEmVVQnwCJ-Q5Hqwf4O8HG5eu6ynbBl8_LzhJXX0OngaI4GRUVF0fhT17S-Fnmo9tS9c&amp;refId=lbnt2cNJFf5kM%2FxHsC7d9A%3D%3D&amp;trackingId=qX89QF2WypEYi9xm3e%2Fr5w%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>JUNIOR EMBEDDED ENGINEER - AGRICULTURAL AUTOMATION (32478)</t>
+          <t>Especialista I Em Desenvolvimento De Software</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bosch Brasil</t>
+          <t>TOTVS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Curitiba e Região (Presencial)</t>
+          <t>Joinville, Santa Catarina, Brasil (Remoto)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4308286750/?eBP=CwEAAAGaAxqMy1r--t-Cn-YyDCzi5R5cFV9g8hK23HqxZjBEBcMBRfE_MS50i4k7WJnM4Cqxv8HfBULWuITTrwNk-XtVMQ6oq84EjHnvnX9mVmaIJ9zzr0gBp8UBv09wPrxnBa1oA_RQWsNGfuezrtm5zb5wZOei91sSwpdZQPX4MRQ3aQAVoX5MGkIdF-5xXnDFHjks-DnLVgI_C2QGSuJlaEMHiRp-uA46z6lpPK-MjjEhu5-npcCFijX-9do4OtuOJeJkGXKeJgXCnHq0_ACdDxJxXd3xfCrPAKHi9hiEIdjR7AGcxp9cBNItpM94rTMwqRDjt11j8_niAa_kPi7qL9MS8WOLT9ov82kwdhQ-ZL5QR27ripcnk2BbWYmTS__Jvjt7EkZbORWxVgvFCF9OZp2tRaMbn6r7IvYNZAA9k8jY6g3S6XaXI6I5-LhtJ8fMuteNwGBhTrJLTKErCVj_qsoF8mUumXBxm07oFxbmVKrChjTgHJRT-Tsb2ItvvTeVJxVJBtI&amp;refId=KljewT48X7gbgzXncwajHQ%3D%3D&amp;trackingId=99ZyDhRK02VoWXt%2F%2BxOytg%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4314916144/?eBP=CwEAAAGaA23jKrrhFD2-P3tQpLlx15pMo-3V0UkGnxIfI4jeX_sNd4LKZlLTu68v3eNAC93DpnZ0I3yaENP2azOhIM2CkHLPfs4pv18nre7XOZBQQFKtttG-SarwqidlUvb624P6ncO9FPDKNtEGMvPQperDwmYXYCPwEcWqzLJ3L9yYFjbbvdp3XQ0moKNqD4pGEu7qbfnetBFXic2-KR3XM7LqwplMNSE8uotnaoCZGgVjsvaVbgqUv4eS8BUjnTQcRob7BadRqwaj_aKdc-YptXQl6KNKq3XxluF8aLf56q1BtzJ8TsYZ6psUk1SdHXAvDUiSre8zGZjPto_DNLHmz29DI4hjCHQs1mI3b_womIojIqc0y71M7lmK8IggXOF4JhKsipFIv4n4Sa4sX74GeLn7IzDm3rgfGFWxe6UVqME9kLC-RjLKNQxeePOSotnveS0S20WMU1IlEt6yHXjmJCxUMOb5Ri2ceU8u61bbeLR7rtN-vUncCde0Nzfx-SMlrTcPRjYlZA&amp;refId=lbnt2cNJFf5kM%2FxHsC7d9A%3D%3D&amp;trackingId=%2Fcn6MbQWo9Ui2%2BVsQ7Hkig%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>
@@ -527,73 +527,73 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4317357720/?eBP=CwEAAAGaAxqMywYwv3jqvfBJLoV8Itb2Pqo2abf6heQ5c5SMx928ik9Yo1D6YkaQbjx9cKBpYL6vLZVI1MgPam69uJFSi1MWUocwStvW-c6fXbQwElE3qWcFJXBaMdmYQs0l46Tt_q4DdSvkzqH3gIhwoDcH_2QyRjzD_LgDsrBByTJMMhAtTMdoS_NrBPdMLF3QQo0VGuICgB9iDJlKec_FowIJIg2zLUVdg9FVsNEmI_665R9QlJvxm3-JuIa4u6AMPukLLRtkdaZVXnQVO6UZ7r61omAaDTFFvSd9n2PuJAJ4-XPeh67bSySSNogj5iNETxY7LOCoskNXkgqg7YOtTNOmYbsaw54foTbb3nzXff40edbR4bWcWKo-ljdTPcm-_TSZTS69BhFHEl7LCBqDsr5oF5Df8FkEJzxXQqbZQOEK5wQXH3dXm_cxTwvp4b9kAT8dCCO1de_DvCIDnN_Dd7GDPkJJYc3fq9_r&amp;refId=KljewT48X7gbgzXncwajHQ%3D%3D&amp;trackingId=CENSZRtjNjJY6oTU483yow%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4317357720/?eBP=BUDGET_EXHAUSTED_JOB&amp;refId=lbnt2cNJFf5kM%2FxHsC7d9A%3D%3D&amp;trackingId=d9wtTWEXo9%2FOk1daq33qAQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ANALISTA P&amp;D JR</t>
+          <t>DESENVOLVEDOR DE HARDWARE AUTOMOMOTIVO PLENO | HÍBRIDO (Curitiba)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Honda Brasil</t>
+          <t>Mobi7 Localiza</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sumaré, São Paulo, Brasil (Presencial)</t>
+          <t>Curitiba, Paraná, Brasil (Híbrido)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4298033073/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=KljewT48X7gbgzXncwajHQ%3D%3D&amp;trackingId=mRIsabvEF%2FJjsaBeDPfVdA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4314908154/?eBP=CwEAAAGaA23jKn2vKEFYv3eCW9b3haFSH-J_pM2FHgZ9uWG6UIER-R3u-VEjK3-B1mMn2mjwwY0TAqFs8ZQcR7W1LHY8kTY3KH9Gsrl5G_LH_S4A-sdSRxC65itJWPbYewr78riFtEl2blOXqiQuBeWDZaqwTGdUmrNSTMcxU5p0xfy8lMi5eAsmZXz0d9D4g2AXkId9FjVkMuFscfHl1MZNGQGUFtPFtEH6ECrASI8HjBVW7ZPrjVM2l5iIj_HgqPmqSpHJKenvSPqvToan9gZXyek7qID9RtDzpRsfIbCZayeNcjUkc2EvfArxD679QqJ4cyPEEYMK6XTn5BXfvTT7OMSBAqcrJMq9wRLl6wRg5_NDWXNUTiT2WsLHT5Qo05vl9sJwIawzkBalADdiNPt_qWW93z_-GNsDS0B_ygHgIxiZcyWsDFvKOaNUqc8mAyVbcKcNT8X_GbQsUAGS4OXnQe4_O8FEZ80qTOeakEU&amp;refId=lbnt2cNJFf5kM%2FxHsC7d9A%3D%3D&amp;trackingId=4LZNlHcTmZEWGLTfYj1F0A%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Automation &amp; Systems Engineer - Indaiatuba/SP</t>
+          <t>ANALISTA P&amp;D JR</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>John Deere</t>
+          <t>Honda Brasil</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Indaiatuba, São Paulo, Brasil (Híbrido)</t>
+          <t>Sumaré, São Paulo, Brasil (Presencial)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4299057167/?eBP=CwEAAAGaAxqMywml0xEDbM9ojJLZPjwpFcAGGVIHBaYugwF2XkOJHxd72Qmg-KF_2QGiH5-W0DnKra72ep6dst1MQptn22FqMTCA0r8jO9vVTVNPtpEu3eeiico1T8hB4GYiaFUgIBncBvRZ6P21sxJX0spagn-0StV7ykCyTwBAAydciarJze5CC3A2lkeQ7BNRSu1i6hidkDi-kzj4RD04BbH4o6AQKqsFlcIFyxaP7r05kmiGs9lBlfsjqNMpAyZAyb0kLwS3lG7a9Pve6RxUVYHrgNhTy0OlegAPHS5KIq558n8lmvm8kvfSSTKkDOKFvqszA3tKl4dQOP3vMgfDjuOxK_Ch_a7Q5lw9FwAnKICZcYcKMu-VTiNLUjtHwI8mSGAHy3ML0jpT_6iRmKuLsZpcDeVuRGy_BPT-CyCILtAQq6sFo48m7sddfPqM0UM1WgPMq20uz_5QiHZlWNiJSrQH1euwa0UL-Q&amp;refId=KljewT48X7gbgzXncwajHQ%3D%3D&amp;trackingId=oKCS4vg1EcSl16iO91KxSA%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4298033073/?eBP=NOT_ELIGIBLE_FOR_CHARGING&amp;refId=lbnt2cNJFf5kM%2FxHsC7d9A%3D%3D&amp;trackingId=Evv0cGJiO1rylxDcAzbe6Q%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Técnico de Suporte de Produto (CONTROL ROOM – TELEMETRIA TRATORES)</t>
+          <t>JUNIOR EMBEDDED ENGINEER - AGRICULTURAL AUTOMATION (32478)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CNH</t>
+          <t>Bosch Brasil</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Curitiba, Paraná, Brasil (Híbrido)</t>
+          <t>Curitiba e Região (Presencial)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/jobs/view/4314901435/?eBP=CwEAAAGaAxqMy2KYFgkJkq1dcmSQFKsnluds4VOSSdo8bvRN7ZlYiP9ukVLWji-CBGTX4dpO2s5rfkWQKWDvB41PPktvTX4iYRtYU8Nagdl-KimaTKtCsuELZBA77-FEzL_1HJHRYfaxoQm_hqnafdWCBP1M8_ayuaHghEGmdw2b8VFoKwu24-Fe_QMWvCblp7Ny-cl8hg1uK62J2J0BBPOGp8bJhDIPNdiITqZLbkMNl24lP4_8roV1nak0RQ6310twYPQiY4hFjoEcyqCXCTd9zpWtPm2NNDeUBn0elvS-RVDuUvOmLXkkIQigyyIj0O4ucvWeeR4kuD4x2t8kQ3WE9NEx8mBWizsBaQcn6dpz0dQf59AoOFPO6hbl7iHAkcu6JP-gCw3brNhrE94Yv8FZldGGwZ5nfwZe9LIaY_Yxd9nolu7gzzRpVeqqbOjjHEnA3JxWaQKHXx_4KLWPVpDHK2RDyDgX9khDHlLe&amp;refId=KljewT48X7gbgzXncwajHQ%3D%3D&amp;trackingId=SGUGtmSuhUE5gzfJofGlPw%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
+          <t>https://www.linkedin.com/jobs/view/4308286750/?eBP=CwEAAAGaA23jKoHE5TFBkZ-uuDwb60pVomW96MrOjRKYnnBLh6ckli9Tw64g1SUhiP_lLCUct003NbsZCqYyC7T8a0f5FIPF8bEyiakKknGW91EmCp4wSYcI7Bj89TStZCudbdIwcmcULotrQotwmh01BcAju8ACsLZq4-BCceeiaP43w9RagAHvUub5NF9VJUWwh-KenDVVh22SvsWJC1YXSWKSyp3qfhxiqU428dgoec_7gLs_f4jzjW9tQKrEE7eDGZUX4UQ68xocKj2espE52ZMx1Gx3SN5NllObo4gPxFwwIZqFAz7OWBaOVQWPJeaDEOi_5GC6xCTeUSLPGUfErR--gYruPiB5p6niuIn2gTs5kZN9ZAYaaVV61KxAuuW_xNcOAmXe0zxt2gYV-E7Bqxpt87DwDmATTEhaS1GuzivVpxJR_o_iPiEdxgL3MyHqW9RbkQ1w0uo7j_uXZ3qsF22rXOIfpm3ueN5WNaFHVMOJT4CiZBrkS_7Tsr-F5Dx_F29aCn67b7oP&amp;refId=lbnt2cNJFf5kM%2FxHsC7d9A%3D%3D&amp;trackingId=IFgaQoKwqC1bK2bcl1sORQ%3D%3D&amp;trk=flagship3_search_srp_jobs</t>
         </is>
       </c>
     </row>

</xml_diff>